<commit_message>
modifica cálculo de hora de entrada
</commit_message>
<xml_diff>
--- a/QA/Bitacora Pruebas.xlsx
+++ b/QA/Bitacora Pruebas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="68">
   <si>
     <t>Nueva Identificacion</t>
   </si>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -873,9 +873,7 @@
         <v>60</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="E11" s="17" t="s">
-        <v>60</v>
-      </c>
+      <c r="E11" s="17"/>
       <c r="F11" t="s">
         <v>63</v>
       </c>
@@ -888,9 +886,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -900,9 +896,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -912,9 +906,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -924,9 +916,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -936,9 +926,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -948,9 +936,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
@@ -1100,9 +1086,7 @@
         <v>60</v>
       </c>
       <c r="D31" s="13"/>
-      <c r="E31" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="E31" s="20"/>
       <c r="F31" t="s">
         <v>65</v>
       </c>
@@ -1151,9 +1135,7 @@
       <c r="D34" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1165,9 +1147,7 @@
       <c r="D35" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -1177,9 +1157,7 @@
         <v>7</v>
       </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E36" s="4"/>
       <c r="F36" t="s">
         <v>63</v>
       </c>
@@ -1192,9 +1170,7 @@
         <v>7</v>
       </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -1204,9 +1180,7 @@
         <v>7</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1221,9 +1195,7 @@
       <c r="D39" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1235,9 +1207,7 @@
       <c r="D40" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1263,9 +1233,7 @@
       <c r="D42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1277,9 +1245,7 @@
       <c r="D43" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1336,7 +1302,9 @@
       <c r="D47" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="4"/>
+      <c r="E47" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -1404,6 +1372,9 @@
       <c r="D52" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E52" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
@@ -1414,9 +1385,7 @@
         <v>60</v>
       </c>
       <c r="D53" s="19"/>
-      <c r="E53" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="E53" s="20"/>
     </row>
     <row r="54" spans="1:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
@@ -1428,9 +1397,6 @@
       <c r="D54" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
@@ -1442,9 +1408,6 @@
       <c r="D55" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E55" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
@@ -1456,9 +1419,6 @@
       <c r="D56" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E56" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -1467,9 +1427,6 @@
       <c r="C57" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
@@ -1481,9 +1438,6 @@
       <c r="D58" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
@@ -1495,9 +1449,6 @@
       <c r="D59" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E59" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
@@ -1509,9 +1460,6 @@
       <c r="D60" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E60" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
@@ -1523,9 +1471,6 @@
       <c r="D61" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -1534,9 +1479,6 @@
       <c r="C62" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
@@ -1548,9 +1490,6 @@
       <c r="D63" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E63" s="12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
@@ -1562,11 +1501,8 @@
       <c r="D64" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>10</v>
       </c>
@@ -1576,11 +1512,8 @@
       <c r="D65" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E65" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>48</v>
       </c>
@@ -1590,11 +1523,8 @@
       <c r="D66" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>52</v>
       </c>
@@ -1604,11 +1534,8 @@
       <c r="D67" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E67" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>12</v>
       </c>
@@ -1618,11 +1545,8 @@
       <c r="D68" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E68" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>49</v>
       </c>
@@ -1632,11 +1556,8 @@
       <c r="D69" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>50</v>
       </c>
@@ -1644,9 +1565,6 @@
         <v>7</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E70" s="12" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>